<commit_message>
Modification schéma et description du flux 2af2c9528341050e130f479296b2112805c50d2a
</commit_message>
<xml_diff>
--- a/21-change-_count=0-for-summary=count/ig/StructureDefinition-oncofair-medicationadministration-component.xlsx
+++ b/21-change-_count=0-for-summary=count/ig/StructureDefinition-oncofair-medicationadministration-component.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2449" uniqueCount="456">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2449" uniqueCount="451">
   <si>
     <t>Property</t>
   </si>
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-09-30T07:50:34+00:00</t>
+    <t>2024-12-31T13:02:34+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -1412,23 +1412,7 @@
     <t>Quantity actually administered to the patient or planned to be administered</t>
   </si>
   <si>
-    <t>The comparator is not used on a SimpleQuantity</t>
-  </si>
-  <si>
-    <t>The context of use may frequently define what kind of quantity this is and therefore what kind of units can be used. The context of use may also restrict the values for the comparator.</t>
-  </si>
-  <si>
-    <t>ele-1:All FHIR elements must have a @value or children {hasValue() or (children().count() &gt; id.count())}
-qty-3:If a code for the unit is present, the system SHALL also be present {code.empty() or system.exists()}sqty-1:The comparator is not used on a SimpleQuantity {comparator.empty()}</t>
-  </si>
-  <si>
     <t>quantiteAdministree</t>
-  </si>
-  <si>
-    <t>n/a,PQ, IVL&lt;PQ&gt;, MO, CO, depending on the values</t>
-  </si>
-  <si>
-    <t>SN (see also Range) or CQ</t>
   </si>
   <si>
     <t>MedicationAdministration.eventHistory</t>
@@ -9280,10 +9264,10 @@
         <v>443</v>
       </c>
       <c r="M65" t="s" s="2">
-        <v>444</v>
+        <v>435</v>
       </c>
       <c r="N65" t="s" s="2">
-        <v>445</v>
+        <v>436</v>
       </c>
       <c r="O65" s="2"/>
       <c r="P65" t="s" s="2">
@@ -9342,13 +9326,13 @@
         <v>89</v>
       </c>
       <c r="AI65" t="s" s="2">
-        <v>20</v>
+        <v>400</v>
       </c>
       <c r="AJ65" t="s" s="2">
-        <v>446</v>
+        <v>101</v>
       </c>
       <c r="AK65" t="s" s="2">
-        <v>447</v>
+        <v>444</v>
       </c>
       <c r="AL65" t="s" s="2">
         <v>20</v>
@@ -9357,18 +9341,18 @@
         <v>20</v>
       </c>
       <c r="AN65" t="s" s="2">
-        <v>448</v>
+        <v>439</v>
       </c>
       <c r="AO65" t="s" s="2">
-        <v>449</v>
+        <v>440</v>
       </c>
     </row>
     <row r="66" hidden="true">
       <c r="A66" t="s" s="2">
-        <v>450</v>
+        <v>445</v>
       </c>
       <c r="B66" t="s" s="2">
-        <v>450</v>
+        <v>445</v>
       </c>
       <c r="C66" s="2"/>
       <c r="D66" t="s" s="2">
@@ -9391,16 +9375,16 @@
         <v>20</v>
       </c>
       <c r="K66" t="s" s="2">
-        <v>451</v>
+        <v>446</v>
       </c>
       <c r="L66" t="s" s="2">
-        <v>452</v>
+        <v>447</v>
       </c>
       <c r="M66" t="s" s="2">
-        <v>453</v>
+        <v>448</v>
       </c>
       <c r="N66" t="s" s="2">
-        <v>454</v>
+        <v>449</v>
       </c>
       <c r="O66" s="2"/>
       <c r="P66" t="s" s="2">
@@ -9450,7 +9434,7 @@
         <v>20</v>
       </c>
       <c r="AF66" t="s" s="2">
-        <v>450</v>
+        <v>445</v>
       </c>
       <c r="AG66" t="s" s="2">
         <v>78</v>
@@ -9474,7 +9458,7 @@
         <v>20</v>
       </c>
       <c r="AN66" t="s" s="2">
-        <v>455</v>
+        <v>450</v>
       </c>
       <c r="AO66" t="s" s="2">
         <v>20</v>

</xml_diff>